<commit_message>
export latest mex files to xlsx. update segments and articles_db.
</commit_message>
<xml_diff>
--- a/data/coded_segments/md_2_2.xlsx
+++ b/data/coded_segments/md_2_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/amr-db/data/coded_segments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4C0164A-0B71-EF45-A681-7295AFFD0885}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A42ABF22-5AC5-7D47-8536-CD88A4939ED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="517">
   <si>
     <t>Color</t>
   </si>
@@ -1538,6 +1538,63 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>1: 3713</t>
+  </si>
+  <si>
+    <t>1: 3733</t>
+  </si>
+  <si>
+    <t>Clostridium difficile</t>
+  </si>
+  <si>
+    <t>11/8/18 14:04:00</t>
+  </si>
+  <si>
+    <t>1: 1647</t>
+  </si>
+  <si>
+    <t>1: 1668</t>
+  </si>
+  <si>
+    <t>Nocardia transvalensis</t>
+  </si>
+  <si>
+    <t>11/8/18 14:05:00</t>
+  </si>
+  <si>
+    <t>1: 1332</t>
+  </si>
+  <si>
+    <t>1: 1336</t>
+  </si>
+  <si>
+    <t>2007.</t>
+  </si>
+  <si>
+    <t>11/12/18 12:31:00</t>
+  </si>
+  <si>
+    <t>3: 1441</t>
+  </si>
+  <si>
+    <t>3: 1447</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>11/12/18 12:32:00</t>
+  </si>
+  <si>
+    <t>3: 1449</t>
+  </si>
+  <si>
+    <t>3: 1452</t>
+  </si>
+  <si>
+    <t>2013</t>
   </si>
 </sst>
 </file>
@@ -2002,7 +2059,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M144"/>
+  <dimension ref="A1:M149"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7921,6 +7978,211 @@
         <v>493</v>
       </c>
     </row>
+    <row r="145" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A145" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="G145" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="H145" s="3">
+        <v>0</v>
+      </c>
+      <c r="I145" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="J145" s="3">
+        <v>21</v>
+      </c>
+      <c r="K145" s="4">
+        <v>9.3992999999999993E-2</v>
+      </c>
+      <c r="L145" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="M145" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A146" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="G146" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="H146" s="3">
+        <v>0</v>
+      </c>
+      <c r="I146" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="J146" s="3">
+        <v>22</v>
+      </c>
+      <c r="K146" s="4">
+        <v>0.149976</v>
+      </c>
+      <c r="L146" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="M146" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A147" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="H147" s="3">
+        <v>0</v>
+      </c>
+      <c r="I147" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="J147" s="3">
+        <v>5</v>
+      </c>
+      <c r="K147" s="4">
+        <v>2.9302999999999999E-2</v>
+      </c>
+      <c r="L147" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="M147" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A148" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="G148" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="H148" s="3">
+        <v>0</v>
+      </c>
+      <c r="I148" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="J148" s="3">
+        <v>7</v>
+      </c>
+      <c r="K148" s="4">
+        <v>1.8915999999999999E-2</v>
+      </c>
+      <c r="L148" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="M148" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A149" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="H149" s="3">
+        <v>0</v>
+      </c>
+      <c r="I149" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="J149" s="3">
+        <v>4</v>
+      </c>
+      <c r="K149" s="4">
+        <v>1.0808999999999999E-2</v>
+      </c>
+      <c r="L149" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="M149" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Run through with latest mex files
</commit_message>
<xml_diff>
--- a/data/coded_segments/md_2_2.xlsx
+++ b/data/coded_segments/md_2_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/amr-db/data/coded_segments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A42ABF22-5AC5-7D47-8536-CD88A4939ED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1626DA24-CF64-B444-B8D0-BBDD530B57BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="519">
   <si>
     <t>Color</t>
   </si>
@@ -1595,6 +1595,12 @@
   </si>
   <si>
     <t>2013</t>
+  </si>
+  <si>
+    <t>chen</t>
+  </si>
+  <si>
+    <t>1/29/19 16:38:51</t>
   </si>
 </sst>
 </file>
@@ -2059,7 +2065,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M149"/>
+  <dimension ref="A1:M150"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8183,6 +8189,47 @@
         <v>513</v>
       </c>
     </row>
+    <row r="150" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A150" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="H150" s="3">
+        <v>0</v>
+      </c>
+      <c r="I150" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="J150" s="3">
+        <v>4</v>
+      </c>
+      <c r="K150" s="4">
+        <v>1.7903500134276253E-2</v>
+      </c>
+      <c r="L150" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Continue QA and mex file fixes
</commit_message>
<xml_diff>
--- a/data/coded_segments/md_2_2.xlsx
+++ b/data/coded_segments/md_2_2.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmamendelsohn/r_projects/amr-db/data/coded_segments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB38D62C-FE9B-E344-8A4B-135232988C3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C6DB27D-F5EE-6B42-BE03-6360AD56033E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="560" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="MAXQDA 12" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="532">
   <si>
     <t>Color</t>
   </si>
@@ -85,7 +85,7 @@
     <t>mdualeh</t>
   </si>
   <si>
-    <t>06/18/2018 00:07:00</t>
+    <t>6/18/18 00:07:00</t>
   </si>
   <si>
     <t>13898</t>
@@ -100,7 +100,7 @@
     <t>o</t>
   </si>
   <si>
-    <t>06/18/2018 00:08:00</t>
+    <t>6/18/18 00:08:00</t>
   </si>
   <si>
     <t>14100</t>
@@ -118,7 +118,7 @@
     <t>34</t>
   </si>
   <si>
-    <t>06/18/2018 00:36:00</t>
+    <t>6/18/18 00:36:00</t>
   </si>
   <si>
     <t>Patient:Sex</t>
@@ -158,7 +158,7 @@
     <t>February</t>
   </si>
   <si>
-    <t>06/18/2018 00:37:00</t>
+    <t>6/18/18 00:37:00</t>
   </si>
   <si>
     <t>Event year</t>
@@ -185,7 +185,7 @@
     <t>Successful treatment</t>
   </si>
   <si>
-    <t>06/18/2018 01:01:00</t>
+    <t>6/18/18 01:01:00</t>
   </si>
   <si>
     <t>14500</t>
@@ -203,7 +203,7 @@
     <t>Outbreak of a nove</t>
   </si>
   <si>
-    <t>06/18/2018 01:02:00</t>
+    <t>6/18/18 01:02:00</t>
   </si>
   <si>
     <t>14509</t>
@@ -232,7 +232,7 @@
     <t>15</t>
   </si>
   <si>
-    <t>06/18/2018 01:15:00</t>
+    <t>6/18/18 01:15:00</t>
   </si>
   <si>
     <t>2: 2085</t>
@@ -268,7 +268,7 @@
     <t>Colombian</t>
   </si>
   <si>
-    <t>06/18/2018 01:16:00</t>
+    <t>6/18/18 01:16:00</t>
   </si>
   <si>
     <t>2: 2516</t>
@@ -305,7 +305,7 @@
     <t>rifampin</t>
   </si>
   <si>
-    <t>06/18/2018 01:17:00</t>
+    <t>6/18/18 01:17:00</t>
   </si>
   <si>
     <t>2: 5131</t>
@@ -359,7 +359,7 @@
     <t>levels</t>
   </si>
   <si>
-    <t>06/18/2018 01:18:00</t>
+    <t>6/18/18 01:18:00</t>
   </si>
   <si>
     <t>15066</t>
@@ -386,7 +386,7 @@
     <t>An Irish outbreak</t>
   </si>
   <si>
-    <t>06/18/2018 01:23:00</t>
+    <t>6/18/18 01:23:00</t>
   </si>
   <si>
     <t>15459</t>
@@ -413,7 +413,7 @@
     <t>51</t>
   </si>
   <si>
-    <t>06/18/2018 01:24:00</t>
+    <t>6/18/18 01:24:00</t>
   </si>
   <si>
     <t>1: 2978</t>
@@ -455,7 +455,7 @@
     <t>amikacin</t>
   </si>
   <si>
-    <t>06/18/2018 01:30:00</t>
+    <t>6/18/18 01:30:00</t>
   </si>
   <si>
     <t>2: 685</t>
@@ -516,7 +516,7 @@
 Resistant Escheric</t>
   </si>
   <si>
-    <t>06/18/2018 01:31:00</t>
+    <t>6/18/18 01:31:00</t>
   </si>
   <si>
     <t>16225</t>
@@ -545,7 +545,7 @@
 Center</t>
   </si>
   <si>
-    <t>06/18/2018 01:36:00</t>
+    <t>6/18/18 01:36:00</t>
   </si>
   <si>
     <t>2: 1253</t>
@@ -596,7 +596,7 @@
     <t>76</t>
   </si>
   <si>
-    <t>06/18/2018 01:37:00</t>
+    <t>6/18/18 01:37:00</t>
   </si>
   <si>
     <t>2: 2854</t>
@@ -674,7 +674,7 @@
     <t>2: 4096</t>
   </si>
   <si>
-    <t>06/18/2018 01:38:00</t>
+    <t>6/18/18 01:38:00</t>
   </si>
   <si>
     <t>16729</t>
@@ -692,7 +692,7 @@
     <t>Letters to the Editor</t>
   </si>
   <si>
-    <t>06/18/2018 01:39:00</t>
+    <t>6/18/18 01:39:00</t>
   </si>
   <si>
     <t>16802</t>
@@ -734,7 +734,7 @@
     <t>S. marcescens</t>
   </si>
   <si>
-    <t>06/18/2018 01:40:00</t>
+    <t>6/18/18 01:40:00</t>
   </si>
   <si>
     <t>1: 3247</t>
@@ -767,7 +767,7 @@
     <t>Introductio</t>
   </si>
   <si>
-    <t>06/18/2018 01:41:00</t>
+    <t>6/18/18 01:41:00</t>
   </si>
   <si>
     <t>18227</t>
@@ -791,7 +791,7 @@
     <t>girl</t>
   </si>
   <si>
-    <t>06/18/2018 01:42:00</t>
+    <t>6/18/18 01:42:00</t>
   </si>
   <si>
     <t>1: 392</t>
@@ -817,7 +817,7 @@
 Burkholderia pseudomallei infection</t>
   </si>
   <si>
-    <t>06/18/2018 09:18:00</t>
+    <t>6/18/18 09:18:00</t>
   </si>
   <si>
     <t>18631</t>
@@ -844,7 +844,7 @@
     <t>Corynebacterium jeikeium</t>
   </si>
   <si>
-    <t>06/18/2018 09:19:00</t>
+    <t>6/18/18 09:19:00</t>
   </si>
   <si>
     <t>1: 234</t>
@@ -865,7 +865,7 @@
     <t>Germany2</t>
   </si>
   <si>
-    <t>06/18/2018 09:21:00</t>
+    <t>6/18/18 09:21:00</t>
   </si>
   <si>
     <t>Bacteria:Strain</t>
@@ -880,7 +880,7 @@
     <t>1087</t>
   </si>
   <si>
-    <t>06/18/2018 09:22:00</t>
+    <t>6/18/18 09:22:00</t>
   </si>
   <si>
     <t>MIC</t>
@@ -904,7 +904,7 @@
     <t>died</t>
   </si>
   <si>
-    <t>06/18/2018 09:23:00</t>
+    <t>6/18/18 09:23:00</t>
   </si>
   <si>
     <t>19004</t>
@@ -928,7 +928,7 @@
     <t>isolates</t>
   </si>
   <si>
-    <t>06/18/2018 09:24:00</t>
+    <t>6/18/18 09:24:00</t>
   </si>
   <si>
     <t>19120</t>
@@ -988,7 +988,7 @@
     <t>Republic of Korea</t>
   </si>
   <si>
-    <t>06/18/2018 09:25:00</t>
+    <t>6/18/18 09:25:00</t>
   </si>
   <si>
     <t>2: 317</t>
@@ -1019,7 +1019,7 @@
 immunocompetent pregnant woman</t>
   </si>
   <si>
-    <t>06/18/2018 09:27:00</t>
+    <t>6/18/18 09:27:00</t>
   </si>
   <si>
     <t>20046</t>
@@ -1035,7 +1035,7 @@
 Enterobacteriaceae: emergence a</t>
   </si>
   <si>
-    <t>06/18/2018 09:28:00</t>
+    <t>6/18/18 09:28:00</t>
   </si>
   <si>
     <t>20146</t>
@@ -1047,7 +1047,7 @@
     <t>Community-ons</t>
   </si>
   <si>
-    <t>06/18/2018 09:34:00</t>
+    <t>6/18/18 09:34:00</t>
   </si>
   <si>
     <t>20339</t>
@@ -1068,7 +1068,7 @@
     <t>1: 1465</t>
   </si>
   <si>
-    <t>06/18/2018 09:35:00</t>
+    <t>6/18/18 09:35:00</t>
   </si>
   <si>
     <t>1: 1596</t>
@@ -1118,7 +1118,7 @@
 cancer and impli</t>
   </si>
   <si>
-    <t>06/18/2018 09:43:00</t>
+    <t>6/18/18 09:43:00</t>
   </si>
   <si>
     <t>21345</t>
@@ -1130,7 +1130,7 @@
     <t xml:space="preserve"> July</t>
   </si>
   <si>
-    <t>06/18/2018 09:44:00</t>
+    <t>6/18/18 09:44:00</t>
   </si>
   <si>
     <t>1: 1492</t>
@@ -1148,7 +1148,7 @@
     <t>1: 1523</t>
   </si>
   <si>
-    <t>06/18/2018 09:45:00</t>
+    <t>6/18/18 09:45:00</t>
   </si>
   <si>
     <t>1: 1532</t>
@@ -1172,7 +1172,7 @@
 2010</t>
   </si>
   <si>
-    <t>06/18/2018 09:53:00</t>
+    <t>6/18/18 09:53:00</t>
   </si>
   <si>
     <t>21988</t>
@@ -1190,7 +1190,7 @@
 method</t>
   </si>
   <si>
-    <t>06/18/2018 09:55:00</t>
+    <t>6/18/18 09:55:00</t>
   </si>
   <si>
     <t>22167</t>
@@ -1259,7 +1259,7 @@
     <t>public hospital</t>
   </si>
   <si>
-    <t>06/18/2018 09:56:00</t>
+    <t>6/18/18 09:56:00</t>
   </si>
   <si>
     <t>3: 1797</t>
@@ -1328,7 +1328,7 @@
     <t>levofloxacin</t>
   </si>
   <si>
-    <t>06/18/2018 09:57:00</t>
+    <t>6/18/18 09:57:00</t>
   </si>
   <si>
     <t>22707</t>
@@ -1341,7 +1341,7 @@
 producing Klebsiella pneumoniae in Ireland</t>
   </si>
   <si>
-    <t>06/18/2018 11:23:00</t>
+    <t>6/18/18 11:23:00</t>
   </si>
   <si>
     <t>23427</t>
@@ -1354,7 +1354,7 @@
 Klebsiella pneumonia</t>
   </si>
   <si>
-    <t>06/18/2018 11:24:00</t>
+    <t>6/18/18 11:24:00</t>
   </si>
   <si>
     <t>23496</t>
@@ -1383,13 +1383,13 @@
     <t>Taiwan</t>
   </si>
   <si>
-    <t>06/18/2018 11:35:00</t>
+    <t>6/18/18 11:35:00</t>
   </si>
   <si>
     <t>Carbapenem re</t>
   </si>
   <si>
-    <t>06/18/2018 11:36:00</t>
+    <t>6/18/18 11:36:00</t>
   </si>
   <si>
     <t>1: 2512</t>
@@ -1404,7 +1404,7 @@
     <t>Sonia</t>
   </si>
   <si>
-    <t>10/29/2018 11:59:00</t>
+    <t>10/29/18 11:59:00</t>
   </si>
   <si>
     <t>1: 3706</t>
@@ -1416,7 +1416,7 @@
     <t>Korea</t>
   </si>
   <si>
-    <t>10/29/2018 12:26:00</t>
+    <t>10/29/18 12:26:00</t>
   </si>
   <si>
     <t>2: 2356</t>
@@ -1428,7 +1428,7 @@
     <t>ampicillin</t>
   </si>
   <si>
-    <t>10/30/2018 15:55:00</t>
+    <t>10/30/18 15:55:00</t>
   </si>
   <si>
     <t>2: 2382</t>
@@ -1474,7 +1474,7 @@
     <t>moxifloxacin</t>
   </si>
   <si>
-    <t>10/30/2018 15:56:00</t>
+    <t>10/30/18 15:56:00</t>
   </si>
   <si>
     <t>2: 2517</t>
@@ -1525,7 +1525,7 @@
     <t>2: 2400</t>
   </si>
   <si>
-    <t>10/30/2018 15:57:00</t>
+    <t>10/30/18 15:57:00</t>
   </si>
   <si>
     <t>C</t>
@@ -1549,7 +1549,7 @@
     <t>Clostridium difficile</t>
   </si>
   <si>
-    <t>11/08/2018 14:04:00</t>
+    <t>11/8/18 14:04:00</t>
   </si>
   <si>
     <t>1: 1647</t>
@@ -1561,7 +1561,7 @@
     <t>Nocardia transvalensis</t>
   </si>
   <si>
-    <t>11/08/2018 14:05:00</t>
+    <t>11/8/18 14:05:00</t>
   </si>
   <si>
     <t>1: 1332</t>
@@ -1573,7 +1573,7 @@
     <t>2007.</t>
   </si>
   <si>
-    <t>11/12/2018 12:31:00</t>
+    <t>11/12/18 12:31:00</t>
   </si>
   <si>
     <t>3: 1441</t>
@@ -1585,7 +1585,7 @@
     <t>October</t>
   </si>
   <si>
-    <t>11/12/2018 12:32:00</t>
+    <t>11/12/18 12:32:00</t>
   </si>
   <si>
     <t>3: 1449</t>
@@ -1600,7 +1600,46 @@
     <t>chen</t>
   </si>
   <si>
-    <t>01/29/2019 16:38:51</t>
+    <t>1/29/19 16:38:51</t>
+  </si>
+  <si>
+    <t>1: 5402</t>
+  </si>
+  <si>
+    <t>1: 5420</t>
+  </si>
+  <si>
+    <t>Sydney Eye Hospital</t>
+  </si>
+  <si>
+    <t>emmamendelsohn</t>
+  </si>
+  <si>
+    <t>8/22/19 14:16:18</t>
+  </si>
+  <si>
+    <t>1: 5423</t>
+  </si>
+  <si>
+    <t>1: 5428</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>8/22/19 14:16:22</t>
+  </si>
+  <si>
+    <t>1: 5431</t>
+  </si>
+  <si>
+    <t>1: 5439</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>8/22/19 14:16:28</t>
   </si>
 </sst>
 </file>
@@ -1615,19 +1654,16 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF909090"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2068,7 +2104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M150"/>
+  <dimension ref="A1:M153"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8233,6 +8269,129 @@
         <v>518</v>
       </c>
     </row>
+    <row r="151" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A151" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="H151" s="3">
+        <v>0</v>
+      </c>
+      <c r="I151" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="J151" s="3">
+        <v>19</v>
+      </c>
+      <c r="K151" s="4">
+        <v>0.12952484831958552</v>
+      </c>
+      <c r="L151" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="M151" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A152" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="G152" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="H152" s="3">
+        <v>0</v>
+      </c>
+      <c r="I152" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="J152" s="3">
+        <v>6</v>
+      </c>
+      <c r="K152" s="4">
+        <v>4.0902583679869112E-2</v>
+      </c>
+      <c r="L152" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="M152" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A153" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="H153" s="3">
+        <v>0</v>
+      </c>
+      <c r="I153" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="J153" s="3">
+        <v>9</v>
+      </c>
+      <c r="K153" s="4">
+        <v>6.1353875519803668E-2</v>
+      </c>
+      <c r="L153" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>